<commit_message>
Fix types error for zone cells in cities table
</commit_message>
<xml_diff>
--- a/excelReader/cities/DELS_.xlsx
+++ b/excelReader/cities/DELS_.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Санкт-Петербург</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>1-3</t>
-  </si>
-  <si>
-    <t>1,9</t>
   </si>
   <si>
     <t>Выборг</t>
@@ -158,9 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -433,7 +431,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,7 +442,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,10 +505,10 @@
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -533,7 +531,7 @@
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -578,8 +576,8 @@
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
+      <c r="G6" s="2">
+        <v>1.9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -587,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -602,7 +600,7 @@
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bags with numbers in cities name
</commit_message>
<xml_diff>
--- a/excelReader/cities/DELS_.xlsx
+++ b/excelReader/cities/DELS_.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Санкт-Петербург</t>
   </si>
@@ -119,6 +119,21 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Горки-46</t>
+  </si>
+  <si>
+    <t>23 Мая</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>23 область</t>
+  </si>
+  <si>
+    <t>Чемихино</t>
   </si>
 </sst>
 </file>
@@ -431,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -439,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +618,75 @@
         <v>29</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>